<commit_message>
excel all tables in
</commit_message>
<xml_diff>
--- a/output/allbc_sens.xlsx
+++ b/output/allbc_sens.xlsx
@@ -58,19 +58,19 @@
         <v>2.5253839492797852</v>
       </c>
       <c r="B1" s="0">
-        <v>0.051597706973552697</v>
+        <v>0.96670711040496826</v>
       </c>
       <c r="C1" s="0">
         <v>9.7480907440185547</v>
       </c>
       <c r="D1" s="0">
-        <v>0.048414941877126701</v>
+        <v>4.6447315216064453</v>
       </c>
       <c r="E1" s="0">
         <v>5.5604968070983887</v>
       </c>
       <c r="F1" s="0">
-        <v>0.048414941877126701</v>
+        <v>4.6447315216064453</v>
       </c>
     </row>
     <row r="2">
@@ -95,22 +95,22 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.059244722127914401</v>
+        <v>0.93554514646530151</v>
       </c>
       <c r="B3" s="0">
-        <v>0.032009117305278799</v>
+        <v>0.77921265363693237</v>
       </c>
       <c r="C3" s="0">
-        <v>0.060474451631307602</v>
+        <v>5.0259566307067871</v>
       </c>
       <c r="D3" s="0">
-        <v>0.037413988262414898</v>
+        <v>3.6013355255126949</v>
       </c>
       <c r="E3" s="0">
-        <v>0.044072266668081297</v>
+        <v>2.3132750988006592</v>
       </c>
       <c r="F3" s="0">
-        <v>0.039431847631931298</v>
+        <v>2.028793573379517</v>
       </c>
     </row>
     <row r="4">
@@ -175,22 +175,22 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.046035692095756503</v>
+        <v>1.3971821069717409</v>
       </c>
       <c r="B7" s="0">
-        <v>0.057055823504924802</v>
+        <v>0.89828085899353027</v>
       </c>
       <c r="C7" s="0">
-        <v>0.038352426141500501</v>
+        <v>2.6527543067932129</v>
       </c>
       <c r="D7" s="0">
-        <v>0.043900080025196103</v>
+        <v>5.126030445098877</v>
       </c>
       <c r="E7" s="0">
-        <v>0.033729434013366699</v>
+        <v>1.339913129806519</v>
       </c>
       <c r="F7" s="0">
-        <v>0.038728371262550403</v>
+        <v>2.2339012622833252</v>
       </c>
     </row>
     <row r="8">
@@ -363,19 +363,19 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.051596552133560201</v>
+        <v>1.0224477052688601</v>
       </c>
       <c r="B17" s="0">
         <v>0.93371975421905518</v>
       </c>
       <c r="C17" s="0">
-        <v>0.043159361928701401</v>
+        <v>5.5734972953796387</v>
       </c>
       <c r="D17" s="0">
         <v>3.4381766319274898</v>
       </c>
       <c r="E17" s="0">
-        <v>0.044496078044176102</v>
+        <v>2.3733184337615971</v>
       </c>
       <c r="F17" s="0">
         <v>1.6662446260452271</v>

</xml_diff>

<commit_message>
add pvalues to tables
</commit_message>
<xml_diff>
--- a/output/allbc_sens.xlsx
+++ b/output/allbc_sens.xlsx
@@ -115,310 +115,484 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>1.1095730066299441</v>
+        <v>0.011112371459603299</v>
       </c>
       <c r="B4" s="0">
-        <v>2.7187232971191411</v>
+        <v>0</v>
       </c>
       <c r="C4" s="0">
-        <v>1.8455755710601811</v>
+        <v>0.059417165815830203</v>
       </c>
       <c r="D4" s="0">
-        <v>2.7187232971191411</v>
+        <v>0</v>
       </c>
       <c r="E4" s="0">
-        <v>1.617049932479858</v>
+        <v>0.018709603697061501</v>
       </c>
       <c r="F4" s="0">
-        <v>2.0461137294769292</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.4137541651725769</v>
+        <v>1.1095730066299441</v>
       </c>
       <c r="B5" s="0">
-        <v>1.9976567029953001</v>
+        <v>1.46378481388092</v>
       </c>
       <c r="C5" s="0">
-        <v>0.627419114112854</v>
+        <v>1.8455755710601811</v>
       </c>
       <c r="D5" s="0">
-        <v>1.9976567029953001</v>
+        <v>2.7187232971191411</v>
       </c>
       <c r="E5" s="0">
-        <v>0.41989445686340332</v>
+        <v>1.617049932479858</v>
       </c>
       <c r="F5" s="0">
-        <v>0.82744580507278442</v>
+        <v>2.0461137294769292</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>4.773097038269043</v>
+        <v>0.4137541651725769</v>
       </c>
       <c r="B6" s="0">
-        <v>2.3026843070983891</v>
+        <v>0.47923716902732849</v>
       </c>
       <c r="C6" s="0">
-        <v>4.3790645599365234</v>
+        <v>0.627419114112854</v>
       </c>
       <c r="D6" s="0">
-        <v>12.474008560180661</v>
+        <v>1.9976567029953001</v>
       </c>
       <c r="E6" s="0">
-        <v>4.4061336517333984</v>
+        <v>0.41989445686340332</v>
       </c>
       <c r="F6" s="0">
-        <v>6.2210268974304199</v>
+        <v>0.82744580507278442</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>1.3971821069717409</v>
+        <v>0.35525569319725042</v>
       </c>
       <c r="B7" s="0">
-        <v>0.89828085899353027</v>
+        <v>0.1838076859712601</v>
       </c>
       <c r="C7" s="0">
-        <v>2.6527543067932129</v>
+        <v>0.1017122119665146</v>
       </c>
       <c r="D7" s="0">
-        <v>5.126030445098877</v>
+        <v>0.2254223823547363</v>
       </c>
       <c r="E7" s="0">
-        <v>1.339913129806519</v>
+        <v>0.089125752449035603</v>
       </c>
       <c r="F7" s="0">
-        <v>2.2339012622833252</v>
+        <v>0.1174736395478249</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>3.6043698787689209</v>
+        <v>4.773097038269043</v>
       </c>
       <c r="B8" s="0">
-        <v>1.987090945243835</v>
+        <v>2.3026843070983891</v>
       </c>
       <c r="C8" s="0">
-        <v>14.54471015930176</v>
+        <v>4.3790645599365234</v>
       </c>
       <c r="D8" s="0">
-        <v>7.3505969047546387</v>
+        <v>12.474008560180661</v>
       </c>
       <c r="E8" s="0">
-        <v>8.2511138916015625</v>
+        <v>4.4061336517333984</v>
       </c>
       <c r="F8" s="0">
-        <v>4.215613842010498</v>
+        <v>6.2210268974304199</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>1.425473690032959</v>
+        <v>1.3971821069717409</v>
       </c>
       <c r="B9" s="0">
-        <v>0.766093909740448</v>
+        <v>0.89828085899353027</v>
       </c>
       <c r="C9" s="0">
-        <v>6.9596858024597168</v>
+        <v>2.6527543067932129</v>
       </c>
       <c r="D9" s="0">
-        <v>3.4934341907501221</v>
+        <v>5.126030445098877</v>
       </c>
       <c r="E9" s="0">
-        <v>3.581947803497314</v>
+        <v>1.339913129806519</v>
       </c>
       <c r="F9" s="0">
-        <v>1.7967971563339229</v>
+        <v>2.2339012622833252</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>4.9198513031005859</v>
+        <v>0</v>
       </c>
       <c r="B10" s="0">
-        <v>1.36979079246521</v>
+        <v>0.086783342063426999</v>
       </c>
       <c r="C10" s="0">
-        <v>25.395139694213871</v>
+        <v>0.12311917543411249</v>
       </c>
       <c r="D10" s="0">
-        <v>3.5423903465271001</v>
+        <v>0.0046572727151214998</v>
       </c>
       <c r="E10" s="0">
-        <v>13.38780498504639</v>
+        <v>0</v>
       </c>
       <c r="F10" s="0">
-        <v>2.3352499008178711</v>
+        <v>0.019503345713019399</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>3.3602781295776372</v>
+        <v>3.6043698787689209</v>
       </c>
       <c r="B11" s="0">
-        <v>0.35952132940292358</v>
+        <v>1.987090945243835</v>
       </c>
       <c r="C11" s="0">
-        <v>13.58416652679443</v>
+        <v>14.54471015930176</v>
       </c>
       <c r="D11" s="0">
-        <v>1.50055992603302</v>
+        <v>7.3505969047546387</v>
       </c>
       <c r="E11" s="0">
-        <v>6.5723638534545898</v>
+        <v>8.2511138916015625</v>
       </c>
       <c r="F11" s="0">
-        <v>0.84229302406311035</v>
+        <v>4.215613842010498</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>2.7864515781402588</v>
-      </c>
-      <c r="B12" s="0"/>
+        <v>1.425473690032959</v>
+      </c>
+      <c r="B12" s="0">
+        <v>0.766093909740448</v>
+      </c>
       <c r="C12" s="0">
-        <v>9.93505859375</v>
-      </c>
-      <c r="D12" s="0"/>
+        <v>6.9596858024597168</v>
+      </c>
+      <c r="D12" s="0">
+        <v>3.4934341907501221</v>
+      </c>
       <c r="E12" s="0">
-        <v>5.7859630584716797</v>
-      </c>
-      <c r="F12" s="0"/>
+        <v>3.581947803497314</v>
+      </c>
+      <c r="F12" s="0">
+        <v>1.7967971563339229</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>1.004591822624207</v>
-      </c>
-      <c r="B13" s="0"/>
+        <v>0.027894319966435401</v>
+      </c>
+      <c r="B13" s="0">
+        <v>0.1130513697862625</v>
+      </c>
       <c r="C13" s="0">
-        <v>4.6531586647033691</v>
-      </c>
-      <c r="D13" s="0"/>
+        <v>0.044109310954809203</v>
+      </c>
+      <c r="D13" s="0">
+        <v>0.049892276525497402</v>
+      </c>
       <c r="E13" s="0">
-        <v>2.4119231700897221</v>
-      </c>
-      <c r="F13" s="0"/>
+        <v>0.032656762748956701</v>
+      </c>
+      <c r="F13" s="0">
+        <v>0.0559020303189754</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>2.12165355682373</v>
+        <v>4.9198513031005859</v>
       </c>
       <c r="B14" s="0">
-        <v>0.59277732255258664</v>
+        <v>1.36979079246521</v>
       </c>
       <c r="C14" s="0">
-        <v>7.1832585334777832</v>
+        <v>25.395139694213871</v>
       </c>
       <c r="D14" s="0">
-        <v>3.619269087285065</v>
+        <v>3.5423903465271001</v>
       </c>
       <c r="E14" s="0">
-        <v>4.8781552314758301</v>
+        <v>13.38780498504639</v>
       </c>
       <c r="F14" s="0">
-        <v>0.85675207053487801</v>
+        <v>2.3352499008178711</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.71570700407028198</v>
+        <v>3.3602781295776372</v>
       </c>
       <c r="B15" s="0">
-        <v>8.7275717222399998e-06</v>
+        <v>0.35952132940292358</v>
       </c>
       <c r="C15" s="0">
-        <v>3.9707100391387939</v>
+        <v>13.58416652679443</v>
       </c>
       <c r="D15" s="0">
-        <v>3.2882598217999999e-05</v>
+        <v>1.50055992603302</v>
       </c>
       <c r="E15" s="0">
-        <v>2.1100478172302251</v>
+        <v>6.5723638534545898</v>
       </c>
       <c r="F15" s="0">
-        <v>1.19337901057e-05</v>
+        <v>0.84229302406311035</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>2.6383829116821289</v>
+        <v>0.13527610898017881</v>
       </c>
       <c r="B16" s="0">
-        <v>2.1653554439544682</v>
+        <v>0.1687266081571579</v>
       </c>
       <c r="C16" s="0">
-        <v>11.7394905090332</v>
+        <v>0.055561855435371399</v>
       </c>
       <c r="D16" s="0">
-        <v>7.2753944396972656</v>
+        <v>0.069282233715057401</v>
       </c>
       <c r="E16" s="0">
-        <v>5.2473974227905273</v>
+        <v>0.036965642124414402</v>
       </c>
       <c r="F16" s="0">
-        <v>4.0558185577392578</v>
+        <v>0.096722982823848697</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>1.0224477052688601</v>
-      </c>
-      <c r="B17" s="0">
-        <v>0.93371975421905518</v>
-      </c>
+        <v>2.7864515781402588</v>
+      </c>
+      <c r="B17" s="0"/>
       <c r="C17" s="0">
-        <v>5.5734972953796387</v>
-      </c>
-      <c r="D17" s="0">
-        <v>3.4381766319274898</v>
-      </c>
+        <v>9.93505859375</v>
+      </c>
+      <c r="D17" s="0"/>
       <c r="E17" s="0">
-        <v>2.3733184337615971</v>
-      </c>
-      <c r="F17" s="0">
-        <v>1.6662446260452271</v>
-      </c>
+        <v>5.7859630584716797</v>
+      </c>
+      <c r="F17" s="0"/>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>2.3691895008087158</v>
-      </c>
-      <c r="B18" s="0">
-        <v>2.6808581352233891</v>
-      </c>
+        <v>1.004591822624207</v>
+      </c>
+      <c r="B18" s="0"/>
       <c r="C18" s="0">
-        <v>9.0459194183349609</v>
-      </c>
-      <c r="D18" s="0">
-        <v>10.48870849609375</v>
-      </c>
+        <v>4.6531586647033691</v>
+      </c>
+      <c r="D18" s="0"/>
       <c r="E18" s="0">
-        <v>4.7231655120849609</v>
-      </c>
-      <c r="F18" s="0">
-        <v>6.4097065925598136</v>
-      </c>
+        <v>2.4119231700897221</v>
+      </c>
+      <c r="F18" s="0"/>
     </row>
     <row r="19">
       <c r="A19" s="0">
+        <v>0.036058511584997198</v>
+      </c>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0">
+        <v>0.043655741959810299</v>
+      </c>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0">
+        <v>0.036738857626914999</v>
+      </c>
+      <c r="F19" s="0"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>2.389339685440063</v>
+      </c>
+      <c r="B20" s="0">
+        <v>2.6628162860870361</v>
+      </c>
+      <c r="C20" s="0">
+        <v>8.897038459777832</v>
+      </c>
+      <c r="D20" s="0">
+        <v>10.603757858276371</v>
+      </c>
+      <c r="E20" s="0">
+        <v>5.3357529640197754</v>
+      </c>
+      <c r="F20" s="0">
+        <v>5.7814178466796884</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>0.85868531465530396</v>
+      </c>
+      <c r="B21" s="0">
+        <v>1.090346574783325</v>
+      </c>
+      <c r="C21" s="0">
+        <v>4.3489298820495614</v>
+      </c>
+      <c r="D21" s="0">
+        <v>5.0070343017578134</v>
+      </c>
+      <c r="E21" s="0">
+        <v>2.2671339511871338</v>
+      </c>
+      <c r="F21" s="0">
+        <v>2.526105403900146</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>0.0564689859747887</v>
+      </c>
+      <c r="B22" s="0">
+        <v>0.067241184413433103</v>
+      </c>
+      <c r="C22" s="0">
+        <v>0.052046716213226298</v>
+      </c>
+      <c r="D22" s="0">
+        <v>0.0449030511081219</v>
+      </c>
+      <c r="E22" s="0">
+        <v>0.0402539968490601</v>
+      </c>
+      <c r="F22" s="0">
+        <v>0.047964621335268</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>2.6383829116821289</v>
+      </c>
+      <c r="B23" s="0">
+        <v>2.1653554439544682</v>
+      </c>
+      <c r="C23" s="0">
+        <v>11.7394905090332</v>
+      </c>
+      <c r="D23" s="0">
+        <v>7.2753944396972656</v>
+      </c>
+      <c r="E23" s="0">
+        <v>5.2473974227905273</v>
+      </c>
+      <c r="F23" s="0">
+        <v>4.0558185577392578</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>2.6383829116821289</v>
+      </c>
+      <c r="B24" s="0">
+        <v>0.93371975421905518</v>
+      </c>
+      <c r="C24" s="0">
+        <v>11.7394905090332</v>
+      </c>
+      <c r="D24" s="0">
+        <v>3.4381766319274898</v>
+      </c>
+      <c r="E24" s="0">
+        <v>5.2473974227905273</v>
+      </c>
+      <c r="F24" s="0">
+        <v>1.6662446260452271</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>2.6383829116821289</v>
+      </c>
+      <c r="B25" s="0">
+        <v>0.1229164302349091</v>
+      </c>
+      <c r="C25" s="0">
+        <v>11.7394905090332</v>
+      </c>
+      <c r="D25" s="0">
+        <v>0.054314546287059798</v>
+      </c>
+      <c r="E25" s="0">
+        <v>5.2473974227905273</v>
+      </c>
+      <c r="F25" s="0">
+        <v>0.049438711255788803</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>2.3691895008087158</v>
+      </c>
+      <c r="B26" s="0">
+        <v>2.6808581352233891</v>
+      </c>
+      <c r="C26" s="0">
+        <v>9.0459194183349609</v>
+      </c>
+      <c r="D26" s="0">
+        <v>10.48870849609375</v>
+      </c>
+      <c r="E26" s="0">
+        <v>4.7231655120849609</v>
+      </c>
+      <c r="F26" s="0">
+        <v>6.4097065925598136</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
         <v>0.90667265653610229</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B27" s="0">
         <v>1.2480931282043459</v>
       </c>
-      <c r="C19" s="0">
+      <c r="C27" s="0">
         <v>4.3858423233032227</v>
       </c>
-      <c r="D19" s="0">
+      <c r="D27" s="0">
         <v>5.249758243560791</v>
       </c>
-      <c r="E19" s="0">
+      <c r="E27" s="0">
         <v>2.3435544967651372</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F27" s="0">
         <v>2.6410386562347412</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>0.070756323635578197</v>
+      </c>
+      <c r="B28" s="0">
+        <v>0.10205239057540889</v>
+      </c>
+      <c r="C28" s="0">
+        <v>0.050912801176309599</v>
+      </c>
+      <c r="D28" s="0">
+        <v>0.051819935441017199</v>
+      </c>
+      <c r="E28" s="0">
+        <v>0.084816873073577895</v>
+      </c>
+      <c r="F28" s="0">
+        <v>0.020750651136040701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some more changes to table
</commit_message>
<xml_diff>
--- a/output/allbc_sens.xlsx
+++ b/output/allbc_sens.xlsx
@@ -55,484 +55,544 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>0.12636555731296539</v>
+        <v>5.5604968070983887</v>
       </c>
       <c r="B1" s="0">
-        <v>0.045029263943433803</v>
+        <v>2.3871057033538818</v>
       </c>
       <c r="C1" s="0">
-        <v>0.13812857866287229</v>
+        <v>9.7480907440185547</v>
       </c>
       <c r="D1" s="0">
-        <v>0.048414941877126701</v>
+        <v>4.6447315216064453</v>
       </c>
       <c r="E1" s="0">
-        <v>0.086773470044136006</v>
+        <v>2.5253839492797852</v>
       </c>
       <c r="F1" s="0">
-        <v>0.051597706973552697</v>
+        <v>0.96670711040496826</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.13596199452877039</v>
+        <v>5.9864659309387207</v>
       </c>
       <c r="B2" s="0">
-        <v>0.12247072160243989</v>
+        <v>5.3182291984558114</v>
       </c>
       <c r="C2" s="0">
-        <v>0.1470357030630112</v>
+        <v>9.7875308990478516</v>
       </c>
       <c r="D2" s="0">
-        <v>0.14765714108943939</v>
+        <v>9.755915641784668</v>
       </c>
       <c r="E2" s="0">
-        <v>0.092296555638313293</v>
+        <v>2.8115313053131099</v>
       </c>
       <c r="F2" s="0">
-        <v>0.087023288011550903</v>
+        <v>2.7417948246002202</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.044072266668081297</v>
+        <v>2.3132750988006592</v>
       </c>
       <c r="B3" s="0">
-        <v>0.039431847631931298</v>
+        <v>2.028793573379517</v>
       </c>
       <c r="C3" s="0">
-        <v>0.060474451631307602</v>
+        <v>5.0259566307067871</v>
       </c>
       <c r="D3" s="0">
-        <v>0.037413988262414898</v>
+        <v>3.6013355255126949</v>
       </c>
       <c r="E3" s="0">
-        <v>0.059244722127914401</v>
+        <v>0.93554514646530151</v>
       </c>
       <c r="F3" s="0">
-        <v>0.032009117305278799</v>
+        <v>0.77921265363693237</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0</v>
+        <v>0.018709603697061501</v>
       </c>
       <c r="B4" s="0">
         <v>0</v>
       </c>
       <c r="C4" s="0">
-        <v>0.0062043797224760004</v>
+        <v>0.059417165815830203</v>
       </c>
       <c r="D4" s="0">
         <v>0</v>
       </c>
       <c r="E4" s="0">
-        <v>0.1708621084690094</v>
+        <v>0.011112371459603299</v>
       </c>
       <c r="F4" s="0">
-        <v>0.0141893057152629</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.1036057323217392</v>
+        <v>1.617049932479858</v>
       </c>
       <c r="B5" s="0">
-        <v>0.11451206356287</v>
+        <v>2.0461137294769292</v>
       </c>
       <c r="C5" s="0">
-        <v>0.110483281314373</v>
+        <v>1.8455755710601811</v>
       </c>
       <c r="D5" s="0">
-        <v>0.12651921808719641</v>
+        <v>2.7187232971191411</v>
       </c>
       <c r="E5" s="0">
-        <v>0.099347189068794306</v>
+        <v>1.1095730066299441</v>
       </c>
       <c r="F5" s="0">
-        <v>0.097613118588924394</v>
+        <v>1.46378481388092</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.044696431607008001</v>
+        <v>0.41989445686340332</v>
       </c>
       <c r="B6" s="0">
-        <v>0.043288793414831203</v>
+        <v>0.82744580507278442</v>
       </c>
       <c r="C6" s="0">
-        <v>0.047116104513406802</v>
+        <v>0.627419114112854</v>
       </c>
       <c r="D6" s="0">
-        <v>0.050553500652313198</v>
+        <v>1.9976567029953001</v>
       </c>
       <c r="E6" s="0">
-        <v>0.055597618222236599</v>
+        <v>0.4137541651725769</v>
       </c>
       <c r="F6" s="0">
-        <v>0.051612280309200301</v>
+        <v>0.47923716902732849</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.061488322913646698</v>
+        <v>0.089125752449035603</v>
       </c>
       <c r="B7" s="0">
-        <v>0.0149503648281097</v>
+        <v>0.1174736395478249</v>
       </c>
       <c r="C7" s="0">
-        <v>0.055263452231884003</v>
+        <v>0.1017122119665146</v>
       </c>
       <c r="D7" s="0">
-        <v>0.042956911027431502</v>
+        <v>0.2254223823547363</v>
       </c>
       <c r="E7" s="0">
-        <v>0.11696202307939529</v>
+        <v>0.35525569319725042</v>
       </c>
       <c r="F7" s="0">
-        <v>0.094544097781181294</v>
+        <v>0.1838076859712601</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.099692165851593004</v>
+        <v>4.4061336517333984</v>
       </c>
       <c r="B8" s="0">
-        <v>0.13170374929904941</v>
+        <v>6.2210268974304199</v>
       </c>
       <c r="C8" s="0">
-        <v>0.084695793688297299</v>
+        <v>4.3790645599365234</v>
       </c>
       <c r="D8" s="0">
-        <v>0.1617773920297623</v>
+        <v>12.474008560180661</v>
       </c>
       <c r="E8" s="0">
-        <v>0.13118936121463781</v>
+        <v>4.773097038269043</v>
       </c>
       <c r="F8" s="0">
-        <v>0.089120998978614793</v>
+        <v>2.3026843070983891</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0.033729434013366699</v>
+        <v>1.339913129806519</v>
       </c>
       <c r="B9" s="0">
-        <v>0.038728371262550403</v>
+        <v>2.2339012622833252</v>
       </c>
       <c r="C9" s="0">
-        <v>0.038352426141500501</v>
+        <v>2.6527543067932129</v>
       </c>
       <c r="D9" s="0">
-        <v>0.043900080025196103</v>
+        <v>5.126030445098877</v>
       </c>
       <c r="E9" s="0">
-        <v>0.046035692095756503</v>
+        <v>1.3971821069717409</v>
       </c>
       <c r="F9" s="0">
-        <v>0.057055823504924802</v>
+        <v>0.89828085899353027</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.037631433457136203</v>
+        <v>0</v>
       </c>
       <c r="B10" s="0">
+        <v>0.019503345713019399</v>
+      </c>
+      <c r="C10" s="0">
+        <v>0.12311917543411249</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0.0046572727151214998</v>
+      </c>
+      <c r="E10" s="0">
         <v>0</v>
       </c>
-      <c r="C10" s="0">
-        <v>0.084828712046146407</v>
-      </c>
-      <c r="D10" s="0">
-        <v>0</v>
-      </c>
-      <c r="E10" s="0">
-        <v>0.0095532452687620995</v>
-      </c>
       <c r="F10" s="0">
-        <v>0.1673649400472641</v>
+        <v>0.086783342063426999</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.17364488542079931</v>
+        <v>8.2511138916015625</v>
       </c>
       <c r="B11" s="0">
-        <v>0.1029663383960724</v>
+        <v>4.215613842010498</v>
       </c>
       <c r="C11" s="0">
-        <v>0.17504540085792539</v>
+        <v>14.54471015930176</v>
       </c>
       <c r="D11" s="0">
-        <v>0.11824943870306021</v>
+        <v>7.3505969047546387</v>
       </c>
       <c r="E11" s="0">
-        <v>0.127987265586853</v>
+        <v>3.6043698787689209</v>
       </c>
       <c r="F11" s="0">
-        <v>0.067590735852718395</v>
+        <v>1.987090945243835</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.063783794641494806</v>
+        <v>3.581947803497314</v>
       </c>
       <c r="B12" s="0">
-        <v>0.0374918468296528</v>
+        <v>1.7967971563339229</v>
       </c>
       <c r="C12" s="0">
-        <v>0.063356123864650699</v>
+        <v>6.9596858024597168</v>
       </c>
       <c r="D12" s="0">
-        <v>0.042370557785034201</v>
+        <v>3.4934341907501221</v>
       </c>
       <c r="E12" s="0">
-        <v>0.089258164167404203</v>
+        <v>1.425473690032959</v>
       </c>
       <c r="F12" s="0">
-        <v>0.036918405443429898</v>
+        <v>0.766093909740448</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.017477329820394499</v>
+        <v>0.032656762748956701</v>
       </c>
       <c r="B13" s="0">
-        <v>0.0097207492217422</v>
+        <v>0.0559020303189754</v>
       </c>
       <c r="C13" s="0">
-        <v>0.0092592593282460993</v>
+        <v>0.044109310954809203</v>
       </c>
       <c r="D13" s="0">
-        <v>0.0163674764335155</v>
+        <v>0.049892276525497402</v>
       </c>
       <c r="E13" s="0">
-        <v>0.15497869253158569</v>
+        <v>0.027894319966435401</v>
       </c>
       <c r="F13" s="0">
-        <v>0.1412004083395004</v>
+        <v>0.1130513697862625</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.14201965928077701</v>
-      </c>
-      <c r="B14" s="0"/>
+        <v>13.38780498504639</v>
+      </c>
+      <c r="B14" s="0">
+        <v>2.3352499008178711</v>
+      </c>
       <c r="C14" s="0">
-        <v>0.1479759365320206</v>
-      </c>
-      <c r="D14" s="0"/>
+        <v>25.395139694213871</v>
+      </c>
+      <c r="D14" s="0">
+        <v>3.5423903465271001</v>
+      </c>
       <c r="E14" s="0">
-        <v>0.1037345007061958</v>
-      </c>
-      <c r="F14" s="0"/>
+        <v>4.9198513031005859</v>
+      </c>
+      <c r="F14" s="0">
+        <v>1.36979079246521</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.0532983988523483</v>
-      </c>
-      <c r="B15" s="0"/>
+        <v>6.5723638534545898</v>
+      </c>
+      <c r="B15" s="0">
+        <v>0.84229302406311035</v>
+      </c>
       <c r="C15" s="0">
-        <v>0.053440123796462999</v>
-      </c>
-      <c r="D15" s="0"/>
+        <v>13.58416652679443</v>
+      </c>
+      <c r="D15" s="0">
+        <v>1.50055992603302</v>
+      </c>
       <c r="E15" s="0">
-        <v>0.069319948554039001</v>
-      </c>
-      <c r="F15" s="0"/>
+        <v>3.3602781295776372</v>
+      </c>
+      <c r="F15" s="0">
+        <v>0.35952132940292358</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.016887186095118498</v>
-      </c>
-      <c r="B16" s="0"/>
+        <v>0.036965642124414402</v>
+      </c>
+      <c r="B16" s="0">
+        <v>0.096722982823848697</v>
+      </c>
       <c r="C16" s="0">
-        <v>0.0122901163995266</v>
-      </c>
-      <c r="D16" s="0"/>
+        <v>0.055561855435371399</v>
+      </c>
+      <c r="D16" s="0">
+        <v>0.069282233715057401</v>
+      </c>
       <c r="E16" s="0">
-        <v>0.14548081159591669</v>
-      </c>
-      <c r="F16" s="0"/>
+        <v>0.13527610898017881</v>
+      </c>
+      <c r="F16" s="0">
+        <v>0.1687266081571579</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.12517888844013211</v>
-      </c>
-      <c r="B17" s="0">
-        <v>0.12737710773944849</v>
-      </c>
+        <v>5.7859630584716797</v>
+      </c>
+      <c r="B17" s="0"/>
       <c r="C17" s="0">
-        <v>0.134881466627121</v>
-      </c>
-      <c r="D17" s="0">
-        <v>0.14078095555305481</v>
-      </c>
+        <v>9.93505859375</v>
+      </c>
+      <c r="D17" s="0"/>
       <c r="E17" s="0">
-        <v>0.084288805723190294</v>
-      </c>
-      <c r="F17" s="0">
-        <v>0.088526733219623593</v>
-      </c>
+        <v>2.7864515781402588</v>
+      </c>
+      <c r="F17" s="0"/>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.045394282788038302</v>
-      </c>
-      <c r="B18" s="0">
-        <v>0.044886264950037003</v>
-      </c>
+        <v>2.4119231700897221</v>
+      </c>
+      <c r="B18" s="0"/>
       <c r="C18" s="0">
-        <v>0.050449974834918997</v>
-      </c>
-      <c r="D18" s="0">
-        <v>0.0470926240086555</v>
-      </c>
+        <v>4.6531586647033691</v>
+      </c>
+      <c r="D18" s="0"/>
       <c r="E18" s="0">
-        <v>0.052193060517311103</v>
-      </c>
-      <c r="F18" s="0">
-        <v>0.051233503967523603</v>
-      </c>
+        <v>1.004591822624207</v>
+      </c>
+      <c r="F18" s="0"/>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.010560381226241601</v>
-      </c>
-      <c r="B19" s="0">
-        <v>0.0104659013450146</v>
-      </c>
+        <v>0.036738857626914999</v>
+      </c>
+      <c r="B19" s="0"/>
       <c r="C19" s="0">
-        <v>0.017799075692892099</v>
-      </c>
-      <c r="D19" s="0">
-        <v>0.0062797013670206001</v>
-      </c>
+        <v>0.043655741959810299</v>
+      </c>
+      <c r="D19" s="0"/>
       <c r="E19" s="0">
-        <v>0.13597281277179721</v>
-      </c>
-      <c r="F19" s="0">
-        <v>0.1181400939822197</v>
-      </c>
+        <v>0.036058511584997198</v>
+      </c>
+      <c r="F19" s="0"/>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.1235839501023293</v>
+        <v>5.3357529640197754</v>
       </c>
       <c r="B20" s="0">
-        <v>0.10980309545993799</v>
+        <v>5.7814178466796884</v>
       </c>
       <c r="C20" s="0">
-        <v>0.15277692675590521</v>
+        <v>8.897038459777832</v>
       </c>
       <c r="D20" s="0">
-        <v>0.12162149697542191</v>
+        <v>10.603757858276371</v>
       </c>
       <c r="E20" s="0">
-        <v>0.089088521897792802</v>
+        <v>2.389339685440063</v>
       </c>
       <c r="F20" s="0">
-        <v>0.08082165569067</v>
+        <v>2.6628162860870361</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.1235839501023293</v>
+        <v>2.2671339511871338</v>
       </c>
       <c r="B21" s="0">
-        <v>0.043957620859146097</v>
+        <v>2.526105403900146</v>
       </c>
       <c r="C21" s="0">
-        <v>0.15277692675590521</v>
+        <v>4.3489298820495614</v>
       </c>
       <c r="D21" s="0">
-        <v>0.045712232589721701</v>
+        <v>5.0070343017578134</v>
       </c>
       <c r="E21" s="0">
-        <v>0.089088521897792802</v>
+        <v>0.85868531465530396</v>
       </c>
       <c r="F21" s="0">
-        <v>0.051078137010335901</v>
+        <v>1.090346574783325</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.1235839501023293</v>
+        <v>0.0402539968490601</v>
       </c>
       <c r="B22" s="0">
-        <v>0.0305662807077169</v>
+        <v>0.047964621335268</v>
       </c>
       <c r="C22" s="0">
-        <v>0.15277692675590521</v>
+        <v>0.052046716213226298</v>
       </c>
       <c r="D22" s="0">
-        <v>0.016634367406368301</v>
+        <v>0.0449030511081219</v>
       </c>
       <c r="E22" s="0">
-        <v>0.089088521897792802</v>
+        <v>0.0564689859747887</v>
       </c>
       <c r="F22" s="0">
-        <v>0.1503686457872391</v>
+        <v>0.067241184413433103</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.1123915687203407</v>
+        <v>5.2473974227905273</v>
       </c>
       <c r="B23" s="0">
-        <v>0.12743611633777621</v>
+        <v>4.0558185577392578</v>
       </c>
       <c r="C23" s="0">
-        <v>0.1362168341875076</v>
+        <v>11.7394905090332</v>
       </c>
       <c r="D23" s="0">
-        <v>0.13417588174343109</v>
+        <v>7.2753944396972656</v>
       </c>
       <c r="E23" s="0">
-        <v>0.091077961027622195</v>
+        <v>2.6383829116821289</v>
       </c>
       <c r="F23" s="0">
-        <v>0.085369579493999495</v>
+        <v>2.1653554439544682</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.057841815054416698</v>
+        <v>5.2473974227905273</v>
       </c>
       <c r="B24" s="0">
-        <v>0.044944088906049701</v>
+        <v>1.6662446260452271</v>
       </c>
       <c r="C24" s="0">
-        <v>0.049387026578187901</v>
+        <v>11.7394905090332</v>
       </c>
       <c r="D24" s="0">
-        <v>0.052732232958078398</v>
+        <v>3.4381766319274898</v>
       </c>
       <c r="E24" s="0">
-        <v>0.052658576518297202</v>
+        <v>2.6383829116821289</v>
       </c>
       <c r="F24" s="0">
-        <v>0.052367225289344801</v>
+        <v>0.93371975421905518</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.0398662537336349</v>
+        <v>5.2473974227905273</v>
       </c>
       <c r="B25" s="0">
-        <v>0.0107903182506561</v>
+        <v>0.049438711255788803</v>
       </c>
       <c r="C25" s="0">
-        <v>0.0097688827663659997</v>
+        <v>11.7394905090332</v>
       </c>
       <c r="D25" s="0">
-        <v>0.0203650631010532</v>
+        <v>0.054314546287059798</v>
       </c>
       <c r="E25" s="0">
-        <v>0.11751227825880051</v>
+        <v>2.6383829116821289</v>
       </c>
       <c r="F25" s="0">
-        <v>0.13197025656700129</v>
+        <v>0.1229164302349091</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>4.7231655120849609</v>
+      </c>
+      <c r="B26" s="0">
+        <v>6.4097065925598136</v>
+      </c>
+      <c r="C26" s="0">
+        <v>9.0459194183349609</v>
+      </c>
+      <c r="D26" s="0">
+        <v>10.48870849609375</v>
+      </c>
+      <c r="E26" s="0">
+        <v>2.3691895008087158</v>
+      </c>
+      <c r="F26" s="0">
+        <v>2.6808581352233891</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>2.3435544967651372</v>
+      </c>
+      <c r="B27" s="0">
+        <v>2.6410386562347412</v>
+      </c>
+      <c r="C27" s="0">
+        <v>4.3858423233032227</v>
+      </c>
+      <c r="D27" s="0">
+        <v>5.249758243560791</v>
+      </c>
+      <c r="E27" s="0">
+        <v>0.90667265653610229</v>
+      </c>
+      <c r="F27" s="0">
+        <v>1.2480931282043459</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>0.084816873073577895</v>
+      </c>
+      <c r="B28" s="0">
+        <v>0.020750651136040701</v>
+      </c>
+      <c r="C28" s="0">
+        <v>0.050912801176309599</v>
+      </c>
+      <c r="D28" s="0">
+        <v>0.051819935441017199</v>
+      </c>
+      <c r="E28" s="0">
+        <v>0.070756323635578197</v>
+      </c>
+      <c r="F28" s="0">
+        <v>0.10205239057540889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all fresh results with qaly all the way up to death
</commit_message>
<xml_diff>
--- a/output/allbc_sens.xlsx
+++ b/output/allbc_sens.xlsx
@@ -55,562 +55,562 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>5.5832858085632324</v>
+        <v>5.6936688423156738</v>
       </c>
       <c r="B1" s="0">
-        <v>2.3223311901092529</v>
+        <v>2.3200821876525879</v>
       </c>
       <c r="C1" s="0">
-        <v>9.7492303848266602</v>
+        <v>11.61890888214111</v>
       </c>
       <c r="D1" s="0">
-        <v>4.5880417823791504</v>
+        <v>5.4856686592102051</v>
       </c>
       <c r="E1" s="0">
-        <v>2.5861110687255859</v>
+        <v>2.6043884754180908</v>
       </c>
       <c r="F1" s="0">
-        <v>0.96727114915847778</v>
+        <v>0.97747862339019775</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>6.0214600563049316</v>
+        <v>6.167360782623291</v>
       </c>
       <c r="B2" s="0">
-        <v>5.3210029602050781</v>
+        <v>5.349449634552002</v>
       </c>
       <c r="C2" s="0">
-        <v>9.810490608215332</v>
+        <v>11.941177368164061</v>
       </c>
       <c r="D2" s="0">
-        <v>9.7305974960327148</v>
+        <v>10.744668006896971</v>
       </c>
       <c r="E2" s="0">
-        <v>2.8768553733825679</v>
+        <v>2.9073679447174068</v>
       </c>
       <c r="F2" s="0">
-        <v>2.7985694408416748</v>
+        <v>2.7933518886566162</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2.2601370811462398</v>
+        <v>2.347348690032959</v>
       </c>
       <c r="B3" s="0">
-        <v>2.0351531505584721</v>
+        <v>2.037355899810791</v>
       </c>
       <c r="C3" s="0">
-        <v>5.0556368827819824</v>
+        <v>6.1433606147766113</v>
       </c>
       <c r="D3" s="0">
-        <v>3.6014912128448491</v>
+        <v>4.1167144775390634</v>
       </c>
       <c r="E3" s="0">
-        <v>0.93392407894134521</v>
+        <v>0.97081983089447021</v>
       </c>
       <c r="F3" s="0">
-        <v>0.78550070524215698</v>
+        <v>0.81006956100463867</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.018369428813457499</v>
+        <v>0</v>
       </c>
       <c r="B4" s="0">
         <v>0</v>
       </c>
       <c r="C4" s="0">
-        <v>0.0581698603928089</v>
+        <v>0.0621385648846626</v>
       </c>
       <c r="D4" s="0">
         <v>0</v>
       </c>
       <c r="E4" s="0">
-        <v>0.0057829683646560002</v>
+        <v>0.0151944663375616</v>
       </c>
       <c r="F4" s="0">
-        <v>0</v>
+        <v>0.00034017462166960002</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>1.542058944702148</v>
+        <v>1.553696751594543</v>
       </c>
       <c r="B5" s="0">
-        <v>1.797340393066406</v>
+        <v>2.0134937763214111</v>
       </c>
       <c r="C5" s="0">
-        <v>2.1514892578125</v>
+        <v>2.1673402786254878</v>
       </c>
       <c r="D5" s="0">
-        <v>2.5455892086029048</v>
+        <v>2.8024673461914058</v>
       </c>
       <c r="E5" s="0">
-        <v>1.18315052986145</v>
+        <v>1.16715931892395</v>
       </c>
       <c r="F5" s="0">
-        <v>1.5189123153686519</v>
+        <v>1.519812226295471</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.42906677722930908</v>
+        <v>0.39071539044380188</v>
       </c>
       <c r="B6" s="0">
-        <v>0.46664446592330933</v>
+        <v>0.87507694959640503</v>
       </c>
       <c r="C6" s="0">
-        <v>0.7006409764289856</v>
+        <v>0.73528432846069336</v>
       </c>
       <c r="D6" s="0">
-        <v>0.87748396396636963</v>
+        <v>1.960937023162842</v>
       </c>
       <c r="E6" s="0">
-        <v>0.40101528167724609</v>
+        <v>0.42580029368400568</v>
       </c>
       <c r="F6" s="0">
-        <v>0.48490497469902039</v>
+        <v>0.4848768413066864</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.1242771297693253</v>
+        <v>0.087424881756305695</v>
       </c>
       <c r="B7" s="0">
-        <v>0.053860981017351199</v>
+        <v>0.1512643098831177</v>
       </c>
       <c r="C7" s="0">
-        <v>0.0621385648846626</v>
+        <v>0.0759723335504532</v>
       </c>
       <c r="D7" s="0">
-        <v>0.036171901971101802</v>
+        <v>0.20070302486419681</v>
       </c>
       <c r="E7" s="0">
-        <v>0.3448236882686615</v>
+        <v>0.34391653537750239</v>
       </c>
       <c r="F7" s="0">
-        <v>0.15149110555648801</v>
+        <v>0.16101598739624021</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>4.4229464530944824</v>
+        <v>4.4388608932495117</v>
       </c>
       <c r="B8" s="0">
-        <v>6.287360668182373</v>
+        <v>6.579505443572998</v>
       </c>
       <c r="C8" s="0">
-        <v>4.3223605155944824</v>
+        <v>3.8782253265380859</v>
       </c>
       <c r="D8" s="0">
-        <v>12.384659767150881</v>
+        <v>10.84785079956055</v>
       </c>
       <c r="E8" s="0">
-        <v>4.8113279342651367</v>
+        <v>4.8900823593139648</v>
       </c>
       <c r="F8" s="0">
-        <v>2.3673393726348881</v>
+        <v>2.398469209671021</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>1.387123227119446</v>
+        <v>1.6801761388778691</v>
       </c>
       <c r="B9" s="0">
-        <v>2.227155208587646</v>
+        <v>2.2211544513702388</v>
       </c>
       <c r="C9" s="0">
-        <v>2.7012944221496582</v>
+        <v>2.779337882995605</v>
       </c>
       <c r="D9" s="0">
-        <v>5.1633520126342773</v>
+        <v>4.1389718055725098</v>
       </c>
       <c r="E9" s="0">
-        <v>1.4195148944854741</v>
+        <v>1.495702385902405</v>
       </c>
       <c r="F9" s="0">
-        <v>0.90523260831832886</v>
+        <v>0.94071346521377563</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0</v>
+        <v>0.0094114979729055994</v>
       </c>
       <c r="B10" s="0">
-        <v>0.0089579317718744</v>
+        <v>0</v>
       </c>
       <c r="C10" s="0">
-        <v>0.1243369951844215</v>
+        <v>0.17148914933204651</v>
       </c>
       <c r="D10" s="0">
-        <v>0.0152954235672951</v>
+        <v>0.0098528312519193008</v>
       </c>
       <c r="E10" s="0">
         <v>0</v>
       </c>
       <c r="F10" s="0">
-        <v>0.075920335948467296</v>
+        <v>0.084731444716453594</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>8.2853794097900391</v>
+        <v>8.4978046417236328</v>
       </c>
       <c r="B11" s="0">
-        <v>4.2327075004577637</v>
+        <v>4.2927126884460449</v>
       </c>
       <c r="C11" s="0">
-        <v>14.545883178710939</v>
+        <v>17.433322906494141</v>
       </c>
       <c r="D11" s="0">
-        <v>7.3516688346862793</v>
+        <v>8.7125892639160156</v>
       </c>
       <c r="E11" s="0">
-        <v>3.6948153972625728</v>
+        <v>3.694975614547729</v>
       </c>
       <c r="F11" s="0">
-        <v>2.0328965187072749</v>
+        <v>2.0593993663787842</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>3.4856352806091309</v>
+        <v>3.470507144927979</v>
       </c>
       <c r="B12" s="0">
-        <v>1.7476499080657959</v>
+        <v>1.753226161003113</v>
       </c>
       <c r="C12" s="0">
-        <v>6.8759822845458984</v>
+        <v>8.194671630859375</v>
       </c>
       <c r="D12" s="0">
-        <v>3.4499399662017818</v>
+        <v>4.1388387680053711</v>
       </c>
       <c r="E12" s="0">
-        <v>1.426782965660095</v>
+        <v>1.428515672683716</v>
       </c>
       <c r="F12" s="0">
-        <v>0.76618826389312744</v>
+        <v>0.79001426696777344</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.027780927717685699</v>
+        <v>0</v>
       </c>
       <c r="B13" s="0">
-        <v>0.050686020404100397</v>
+        <v>0.0260800551623106</v>
       </c>
       <c r="C13" s="0">
-        <v>0.043542351573705701</v>
+        <v>0.042748611420392997</v>
       </c>
       <c r="D13" s="0">
-        <v>0.0502324514091015</v>
+        <v>0.050345845520496403</v>
       </c>
       <c r="E13" s="0">
-        <v>0.021997958421707198</v>
+        <v>0.0250595305114985</v>
       </c>
       <c r="F13" s="0">
-        <v>0.1037532612681389</v>
+        <v>0.1097630113363266</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>13.39943885803223</v>
+        <v>13.381679534912109</v>
       </c>
       <c r="B14" s="0">
-        <v>2.3677082061767578</v>
+        <v>2.3976233005523682</v>
       </c>
       <c r="C14" s="0">
-        <v>25.384164810180661</v>
+        <v>29.503713607788089</v>
       </c>
       <c r="D14" s="0">
-        <v>3.5470073223114009</v>
+        <v>4.2094178199768066</v>
       </c>
       <c r="E14" s="0">
-        <v>4.9777603149414062</v>
+        <v>5.3405337333679199</v>
       </c>
       <c r="F14" s="0">
-        <v>1.435282826423645</v>
+        <v>1.42705225944519</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>6.5063791275024414</v>
+        <v>7.0147819519042969</v>
       </c>
       <c r="B15" s="0">
-        <v>0.7968747615814209</v>
+        <v>0.79926526546478271</v>
       </c>
       <c r="C15" s="0">
-        <v>13.551328659057621</v>
+        <v>15.926371574401861</v>
       </c>
       <c r="D15" s="0">
-        <v>1.445855975151062</v>
+        <v>1.875824570655823</v>
       </c>
       <c r="E15" s="0">
-        <v>3.3586935997009282</v>
+        <v>3.8059380054473881</v>
       </c>
       <c r="F15" s="0">
-        <v>0.37079387903213501</v>
+        <v>0.36782318353652949</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.036171901971101802</v>
+        <v>0.033904071897268302</v>
       </c>
       <c r="B16" s="0">
-        <v>0.069395624101161998</v>
+        <v>0.054994896054267897</v>
       </c>
       <c r="C16" s="0">
-        <v>0.055675245821475997</v>
+        <v>0.046377141028642703</v>
       </c>
       <c r="D16" s="0">
-        <v>0.052273500710725798</v>
+        <v>0.0647465735673904</v>
       </c>
       <c r="E16" s="0">
-        <v>0.13108062744140631</v>
+        <v>0.1416260302066803</v>
       </c>
       <c r="F16" s="0">
-        <v>0.13040027022361761</v>
+        <v>0.14842952787876129</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>5.8147902488708496</v>
+        <v>5.9229393005371094</v>
       </c>
       <c r="B17" s="0">
-        <v>6.065887451171875</v>
+        <v>5.6020946502685547</v>
       </c>
       <c r="C17" s="0">
-        <v>9.9365062713623047</v>
+        <v>11.8045711517334</v>
       </c>
       <c r="D17" s="0">
-        <v>10.266337394714361</v>
+        <v>12.35573768615723</v>
       </c>
       <c r="E17" s="0">
-        <v>2.862336158752441</v>
+        <v>2.8794927597045898</v>
       </c>
       <c r="F17" s="0">
-        <v>3.1478474140167241</v>
+        <v>3.2701313495635991</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>2.3315773010253911</v>
+        <v>2.323607444763184</v>
       </c>
       <c r="B18" s="0">
-        <v>2.4945089817047119</v>
+        <v>2.3922076225280762</v>
       </c>
       <c r="C18" s="0">
-        <v>4.5813112258911133</v>
+        <v>5.4853191375732422</v>
       </c>
       <c r="D18" s="0">
-        <v>4.6661882400512704</v>
+        <v>5.678532600402832</v>
       </c>
       <c r="E18" s="0">
-        <v>1.006637811660767</v>
+        <v>1.0181577205657959</v>
       </c>
       <c r="F18" s="0">
-        <v>1.1025897264480591</v>
+        <v>1.2050132751464839</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.031182674691080998</v>
+        <v>0</v>
       </c>
       <c r="B19" s="0">
-        <v>0.035945117473602302</v>
+        <v>0.046150356531143202</v>
       </c>
       <c r="C19" s="0">
         <v>0.044109310954809203</v>
       </c>
       <c r="D19" s="0">
-        <v>0.043428961187601103</v>
+        <v>0.033110331743955598</v>
       </c>
       <c r="E19" s="0">
-        <v>0.028234492987394302</v>
+        <v>0.031182674691080998</v>
       </c>
       <c r="F19" s="0">
-        <v>0.022564915940165499</v>
+        <v>0.029368409886956201</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>5.3599381446838379</v>
+        <v>5.4807124137878418</v>
       </c>
       <c r="B20" s="0">
-        <v>5.8031654357910156</v>
+        <v>5.9036440849304199</v>
       </c>
       <c r="C20" s="0">
-        <v>8.8905773162841797</v>
+        <v>10.758102416992189</v>
       </c>
       <c r="D20" s="0">
-        <v>10.60992527008057</v>
+        <v>12.485054016113279</v>
       </c>
       <c r="E20" s="0">
-        <v>2.4506127834320068</v>
+        <v>2.46998119354248</v>
       </c>
       <c r="F20" s="0">
-        <v>2.723048210144043</v>
+        <v>2.7395250797271729</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>2.217316865921021</v>
+        <v>2.2481460571289058</v>
       </c>
       <c r="B21" s="0">
-        <v>2.4491453170776372</v>
+        <v>2.4085185527801509</v>
       </c>
       <c r="C21" s="0">
-        <v>4.2900118827819824</v>
+        <v>5.3340492248535156</v>
       </c>
       <c r="D21" s="0">
-        <v>4.9543957710266113</v>
+        <v>5.7138128280639648</v>
       </c>
       <c r="E21" s="0">
-        <v>0.86014640331268311</v>
+        <v>0.87048935890197754</v>
       </c>
       <c r="F21" s="0">
-        <v>1.0903869867324829</v>
+        <v>1.09971022605896</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.038666516542434699</v>
+        <v>0.0094114979729055994</v>
       </c>
       <c r="B22" s="0">
-        <v>0.0410477370023727</v>
+        <v>0.0100918468087912</v>
       </c>
       <c r="C22" s="0">
-        <v>0.051026195287704502</v>
+        <v>0.057716295123100302</v>
       </c>
       <c r="D22" s="0">
-        <v>0.043542351573705701</v>
+        <v>0.0390066914260387</v>
       </c>
       <c r="E22" s="0">
-        <v>0.049892276525497402</v>
+        <v>0.047851230949163402</v>
       </c>
       <c r="F22" s="0">
-        <v>0.058736819773912402</v>
+        <v>0.0621385648846626</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>5.2578716278076172</v>
+        <v>5.1388301849365234</v>
       </c>
       <c r="B23" s="0">
-        <v>4.0744743347167969</v>
+        <v>4.0650792121887207</v>
       </c>
       <c r="C23" s="0">
-        <v>11.754641532897949</v>
+        <v>11.82403469085693</v>
       </c>
       <c r="D23" s="0">
-        <v>7.2866725921630859</v>
+        <v>8.3266792297363281</v>
       </c>
       <c r="E23" s="0">
-        <v>2.6994068622589111</v>
+        <v>2.7171530723571782</v>
       </c>
       <c r="F23" s="0">
-        <v>2.2259418964385991</v>
+        <v>2.2452554702758789</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>2.3146827220916748</v>
+        <v>2.2958559989929199</v>
       </c>
       <c r="B24" s="0">
-        <v>1.5853704214096069</v>
+        <v>1.495477080345154</v>
       </c>
       <c r="C24" s="0">
-        <v>5.5850119590759277</v>
+        <v>5.5858626365661621</v>
       </c>
       <c r="D24" s="0">
-        <v>3.4123992919921879</v>
+        <v>3.640516042709351</v>
       </c>
       <c r="E24" s="0">
-        <v>1.0277343988418579</v>
+        <v>1.0422413349151609</v>
       </c>
       <c r="F24" s="0">
-        <v>0.93528419733047485</v>
+        <v>0.94734293222427368</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.045129831880330998</v>
+        <v>0.056922554969787598</v>
       </c>
       <c r="B25" s="0">
-        <v>0.038326341658830601</v>
+        <v>0.0113391540944576</v>
       </c>
       <c r="C25" s="0">
-        <v>0.055561855435371399</v>
+        <v>0.039573647081852001</v>
       </c>
       <c r="D25" s="0">
-        <v>0.055561855435371399</v>
+        <v>0.025399705395102501</v>
       </c>
       <c r="E25" s="0">
-        <v>0.052160110324621201</v>
+        <v>0.055448465049266801</v>
       </c>
       <c r="F25" s="0">
-        <v>0.1131647601723671</v>
+        <v>0.11463885009288791</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>4.747276782989502</v>
+        <v>4.8467903137207031</v>
       </c>
       <c r="B26" s="0">
-        <v>6.430915355682373</v>
+        <v>6.5609383583068848</v>
       </c>
       <c r="C26" s="0">
-        <v>9.0481033325195312</v>
+        <v>10.61320686340332</v>
       </c>
       <c r="D26" s="0">
-        <v>10.487582206726071</v>
+        <v>12.63347148895264</v>
       </c>
       <c r="E26" s="0">
-        <v>2.4293878078460689</v>
+        <v>2.4750146865844731</v>
       </c>
       <c r="F26" s="0">
-        <v>2.742524385452271</v>
+        <v>2.7291877269744869</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>2.2595479488372798</v>
+        <v>2.3249607086181641</v>
       </c>
       <c r="B27" s="0">
-        <v>2.5943295955657959</v>
+        <v>2.5415868759155269</v>
       </c>
       <c r="C27" s="0">
-        <v>4.3158783912658691</v>
+        <v>5.3689374923706046</v>
       </c>
       <c r="D27" s="0">
-        <v>5.2102189064025879</v>
+        <v>5.9021234512329102</v>
       </c>
       <c r="E27" s="0">
-        <v>0.90668070316314697</v>
+        <v>0.97226804494857788</v>
       </c>
       <c r="F27" s="0">
-        <v>1.2494436502456669</v>
+        <v>1.260570764541626</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.0759723335504532</v>
+        <v>0.064633175730705303</v>
       </c>
       <c r="B28" s="0">
-        <v>0.0193899534642696</v>
+        <v>0</v>
       </c>
       <c r="C28" s="0">
-        <v>0.048758361488580697</v>
+        <v>0.051026195287704502</v>
       </c>
       <c r="D28" s="0">
-        <v>0.053747590631246601</v>
+        <v>0.038779906928539297</v>
       </c>
       <c r="E28" s="0">
-        <v>0.060210909694433198</v>
+        <v>0.073817893862724304</v>
       </c>
       <c r="F28" s="0">
-        <v>0.092414103448391002</v>
+        <v>0.099104203283786801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>